<commit_message>
Add Parameter and Syntax Specifications
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CF2874-3AFC-455B-9982-476BB5E7BCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D29D06-433C-4050-86D7-83C7CD7077DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,45 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Post Number</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>Hashtag 1</t>
-  </si>
-  <si>
-    <t>Hashtag 2</t>
-  </si>
-  <si>
-    <t>Hashtag 3</t>
-  </si>
-  <si>
-    <t>Base Engagement</t>
-  </si>
-  <si>
-    <t>Boosted Engagement</t>
-  </si>
-  <si>
-    <t>Boost Cost</t>
-  </si>
-  <si>
-    <t>Image File</t>
-  </si>
-  <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>Publisher</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Post Number (Integer)</t>
+  </si>
+  <si>
+    <t>Publisher (String)</t>
+  </si>
+  <si>
+    <t>Subject (Government, Violence, Health, Radicalism)</t>
+  </si>
+  <si>
+    <t>Day (Integer, 1-8)</t>
+  </si>
+  <si>
+    <t>Reaction (Happy, Sad, Angry)</t>
+  </si>
+  <si>
+    <t>Hashtag 1 (String)</t>
+  </si>
+  <si>
+    <t>Hashtag 2 (String)</t>
+  </si>
+  <si>
+    <t>Hashtag 3 (String)</t>
+  </si>
+  <si>
+    <t>Base Engagement (Integer)</t>
+  </si>
+  <si>
+    <t>Boosted Engagement (Integer)</t>
+  </si>
+  <si>
+    <t>Boost Cost (Float)</t>
+  </si>
+  <si>
+    <t>Headline (String)</t>
+  </si>
+  <si>
+    <t>Image File Path (String)</t>
+  </si>
+  <si>
+    <t>Warning: do not use commas in string text</t>
   </si>
 </sst>
 </file>
@@ -122,19 +125,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A44B44BB-C124-416A-A5ED-96BB8790C489}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0">
   <autoFilter ref="A1:M4" xr:uid="{A44B44BB-C124-416A-A5ED-96BB8790C489}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A937A89C-83D8-47F8-A939-870491748BB5}" name="Post Number"/>
-    <tableColumn id="2" xr3:uid="{A8EF90EC-7501-4CAC-9D7B-BE5B573D1E94}" name="Publisher"/>
-    <tableColumn id="3" xr3:uid="{872F46ED-9A97-4884-87EA-B74DD8C9F9BF}" name="Subject"/>
-    <tableColumn id="4" xr3:uid="{36B97FA6-B33F-4DE1-B9DC-F0FEA9FE8AE1}" name="Day"/>
-    <tableColumn id="5" xr3:uid="{09621E9C-3C9D-433E-A258-75193CBBC6B5}" name="Reaction"/>
-    <tableColumn id="6" xr3:uid="{672F08D8-8913-457E-AE3B-06C0C51FB77F}" name="Hashtag 1"/>
-    <tableColumn id="7" xr3:uid="{138FDF3D-648F-448D-976E-7FA90153CDBA}" name="Hashtag 2"/>
-    <tableColumn id="8" xr3:uid="{D221DCB3-339D-4547-A686-C0A14B78F5A8}" name="Hashtag 3"/>
-    <tableColumn id="9" xr3:uid="{FA9BCD0A-EFD9-4FA2-9B00-B6D8748094C7}" name="Base Engagement"/>
-    <tableColumn id="10" xr3:uid="{394B2133-9A3B-4549-9628-338B588047E1}" name="Boosted Engagement"/>
-    <tableColumn id="11" xr3:uid="{FB8F38F8-7B80-42B3-BABD-6B09E43B42E7}" name="Boost Cost"/>
-    <tableColumn id="12" xr3:uid="{90123981-6599-4E19-882F-16B99DF735F8}" name="Headline"/>
-    <tableColumn id="13" xr3:uid="{72271049-51D5-47E0-973A-28F53D2C997B}" name="Image File"/>
+    <tableColumn id="1" xr3:uid="{A937A89C-83D8-47F8-A939-870491748BB5}" name="Post Number (Integer)"/>
+    <tableColumn id="2" xr3:uid="{A8EF90EC-7501-4CAC-9D7B-BE5B573D1E94}" name="Publisher (String)"/>
+    <tableColumn id="3" xr3:uid="{872F46ED-9A97-4884-87EA-B74DD8C9F9BF}" name="Subject (Government, Violence, Health, Radicalism)"/>
+    <tableColumn id="4" xr3:uid="{36B97FA6-B33F-4DE1-B9DC-F0FEA9FE8AE1}" name="Day (Integer, 1-8)"/>
+    <tableColumn id="5" xr3:uid="{09621E9C-3C9D-433E-A258-75193CBBC6B5}" name="Reaction (Happy, Sad, Angry)"/>
+    <tableColumn id="6" xr3:uid="{672F08D8-8913-457E-AE3B-06C0C51FB77F}" name="Hashtag 1 (String)"/>
+    <tableColumn id="7" xr3:uid="{138FDF3D-648F-448D-976E-7FA90153CDBA}" name="Hashtag 2 (String)"/>
+    <tableColumn id="8" xr3:uid="{D221DCB3-339D-4547-A686-C0A14B78F5A8}" name="Hashtag 3 (String)"/>
+    <tableColumn id="9" xr3:uid="{FA9BCD0A-EFD9-4FA2-9B00-B6D8748094C7}" name="Base Engagement (Integer)"/>
+    <tableColumn id="10" xr3:uid="{394B2133-9A3B-4549-9628-338B588047E1}" name="Boosted Engagement (Integer)"/>
+    <tableColumn id="11" xr3:uid="{FB8F38F8-7B80-42B3-BABD-6B09E43B42E7}" name="Boost Cost (Float)"/>
+    <tableColumn id="12" xr3:uid="{90123981-6599-4E19-882F-16B99DF735F8}" name="Headline (String)"/>
+    <tableColumn id="13" xr3:uid="{72271049-51D5-47E0-973A-28F53D2C997B}" name="Image File Path (String)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,24 +406,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -429,40 +433,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement CSV Data Parsing
Implement scriptable objects for media posts and importing media post data from CSV file.
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D29D06-433C-4050-86D7-83C7CD7077DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D055FEB-51F1-4588-89F8-99FA8110D3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Post Number (Integer)</t>
   </si>
@@ -67,12 +67,87 @@
   </si>
   <si>
     <t>Warning: do not use commas in string text</t>
+  </si>
+  <si>
+    <t>Pox</t>
+  </si>
+  <si>
+    <t>CYPost</t>
+  </si>
+  <si>
+    <t>Forbees</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Violence</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>KeepThemIn</t>
+  </si>
+  <si>
+    <t>GetsThingsDone</t>
+  </si>
+  <si>
+    <t>InGoodHands</t>
+  </si>
+  <si>
+    <t>Government Popularity All Time High</t>
+  </si>
+  <si>
+    <t>post_001.jpg</t>
+  </si>
+  <si>
+    <t>post_002.jpg</t>
+  </si>
+  <si>
+    <t>post_003.jpg</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>TooSoon</t>
+  </si>
+  <si>
+    <t>SoTragic</t>
+  </si>
+  <si>
+    <t>PrayForThem</t>
+  </si>
+  <si>
+    <t>Child Dies From Riot Injuries</t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>CrappyHealthCare</t>
+  </si>
+  <si>
+    <t>OverpaidIdiots</t>
+  </si>
+  <si>
+    <t>MoneyForWhat</t>
+  </si>
+  <si>
+    <t>Surgeons Walk Out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,13 +177,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,7 +209,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A44B44BB-C124-416A-A5ED-96BB8790C489}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0">
   <autoFilter ref="A1:M4" xr:uid="{A44B44BB-C124-416A-A5ED-96BB8790C489}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A937A89C-83D8-47F8-A939-870491748BB5}" name="Post Number (Integer)"/>
+    <tableColumn id="1" xr3:uid="{A937A89C-83D8-47F8-A939-870491748BB5}" name="Post Number (Integer)" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{A8EF90EC-7501-4CAC-9D7B-BE5B573D1E94}" name="Publisher (String)"/>
     <tableColumn id="3" xr3:uid="{872F46ED-9A97-4884-87EA-B74DD8C9F9BF}" name="Subject (Government, Violence, Health, Radicalism)"/>
     <tableColumn id="4" xr3:uid="{36B97FA6-B33F-4DE1-B9DC-F0FEA9FE8AE1}" name="Day (Integer, 1-8)"/>
@@ -135,7 +219,7 @@
     <tableColumn id="8" xr3:uid="{D221DCB3-339D-4547-A686-C0A14B78F5A8}" name="Hashtag 3 (String)"/>
     <tableColumn id="9" xr3:uid="{FA9BCD0A-EFD9-4FA2-9B00-B6D8748094C7}" name="Base Engagement (Integer)"/>
     <tableColumn id="10" xr3:uid="{394B2133-9A3B-4549-9628-338B588047E1}" name="Boosted Engagement (Integer)"/>
-    <tableColumn id="11" xr3:uid="{FB8F38F8-7B80-42B3-BABD-6B09E43B42E7}" name="Boost Cost (Float)"/>
+    <tableColumn id="11" xr3:uid="{FB8F38F8-7B80-42B3-BABD-6B09E43B42E7}" name="Boost Cost (Float)" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{90123981-6599-4E19-882F-16B99DF735F8}" name="Headline (String)"/>
     <tableColumn id="13" xr3:uid="{72271049-51D5-47E0-973A-28F53D2C997B}" name="Image File Path (String)"/>
   </tableColumns>
@@ -408,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +507,7 @@
     <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -469,6 +553,129 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>75</v>
+      </c>
+      <c r="J2">
+        <v>16000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>117</v>
+      </c>
+      <c r="J3">
+        <v>28000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>156</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>15000</v>
+      </c>
+      <c r="K4" s="2">
+        <v>80</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
@@ -476,8 +683,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Media Post Functionality
Implement post instantiation, post scrolling, and post boosting.
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\Desktop\Computer Science\BGDS Yr-03 Semester 06_Design_Practice_04\Source\Narrative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grayn\OneDrive\Documents\short\Under Choices\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8BC05-C584-4F61-91E9-4C8B3BE79F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F915515-0277-451C-B577-1EA6E55D9F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,6 +1116,12 @@
       <c r="H5" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="I5">
+        <v>75</v>
+      </c>
+      <c r="J5">
+        <v>16000</v>
+      </c>
       <c r="K5" s="1">
         <v>75</v>
       </c>
@@ -1151,6 +1157,12 @@
       <c r="H6" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="I6">
+        <v>117</v>
+      </c>
+      <c r="J6">
+        <v>28000</v>
+      </c>
       <c r="K6" s="1">
         <v>121</v>
       </c>
@@ -1186,6 +1198,12 @@
       <c r="H7" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>15000</v>
+      </c>
       <c r="K7" s="1">
         <v>131</v>
       </c>
@@ -1221,6 +1239,12 @@
       <c r="H8" s="7" t="s">
         <v>90</v>
       </c>
+      <c r="I8">
+        <v>75</v>
+      </c>
+      <c r="J8">
+        <v>16000</v>
+      </c>
       <c r="K8" s="1">
         <v>98</v>
       </c>
@@ -1256,6 +1280,12 @@
       <c r="H9" s="7" t="s">
         <v>90</v>
       </c>
+      <c r="I9">
+        <v>117</v>
+      </c>
+      <c r="J9">
+        <v>28000</v>
+      </c>
       <c r="K9" s="1">
         <v>132</v>
       </c>
@@ -1291,6 +1321,12 @@
       <c r="H10" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10">
+        <v>15000</v>
+      </c>
       <c r="K10" s="1">
         <v>149</v>
       </c>
@@ -1326,6 +1362,12 @@
       <c r="H11" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="I11">
+        <v>75</v>
+      </c>
+      <c r="J11">
+        <v>16000</v>
+      </c>
       <c r="K11" s="1">
         <v>89</v>
       </c>
@@ -1361,6 +1403,12 @@
       <c r="H12" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="I12">
+        <v>117</v>
+      </c>
+      <c r="J12">
+        <v>28000</v>
+      </c>
       <c r="K12" s="1">
         <v>69</v>
       </c>
@@ -1396,6 +1444,12 @@
       <c r="H13" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+      <c r="J13">
+        <v>15000</v>
+      </c>
       <c r="K13" s="1">
         <v>50</v>
       </c>
@@ -1431,6 +1485,12 @@
       <c r="H14" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="I14">
+        <v>75</v>
+      </c>
+      <c r="J14">
+        <v>16000</v>
+      </c>
       <c r="K14" s="1">
         <v>134</v>
       </c>
@@ -1466,6 +1526,12 @@
       <c r="H15" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="I15">
+        <v>117</v>
+      </c>
+      <c r="J15">
+        <v>28000</v>
+      </c>
       <c r="K15" s="1">
         <v>78</v>
       </c>
@@ -1501,6 +1567,12 @@
       <c r="H16" s="7" t="s">
         <v>101</v>
       </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <v>15000</v>
+      </c>
       <c r="K16" s="1">
         <v>145</v>
       </c>
@@ -1536,6 +1608,12 @@
       <c r="H17" s="7" t="s">
         <v>101</v>
       </c>
+      <c r="I17">
+        <v>75</v>
+      </c>
+      <c r="J17">
+        <v>16000</v>
+      </c>
       <c r="K17" s="1">
         <v>82</v>
       </c>
@@ -1571,6 +1649,12 @@
       <c r="H18" s="7" t="s">
         <v>103</v>
       </c>
+      <c r="I18">
+        <v>117</v>
+      </c>
+      <c r="J18">
+        <v>28000</v>
+      </c>
       <c r="K18" s="1">
         <v>175</v>
       </c>
@@ -1606,6 +1690,12 @@
       <c r="H19" s="7" t="s">
         <v>103</v>
       </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>15000</v>
+      </c>
       <c r="K19" s="1">
         <v>91</v>
       </c>
@@ -1641,6 +1731,12 @@
       <c r="H20" s="7" t="s">
         <v>106</v>
       </c>
+      <c r="I20">
+        <v>75</v>
+      </c>
+      <c r="J20">
+        <v>16000</v>
+      </c>
       <c r="K20" s="1">
         <v>150</v>
       </c>
@@ -1676,6 +1772,12 @@
       <c r="H21" s="7" t="s">
         <v>106</v>
       </c>
+      <c r="I21">
+        <v>117</v>
+      </c>
+      <c r="J21">
+        <v>28000</v>
+      </c>
       <c r="K21" s="1">
         <v>110</v>
       </c>
@@ -1711,6 +1813,12 @@
       <c r="H22" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <v>15000</v>
+      </c>
       <c r="K22" s="1">
         <v>60</v>
       </c>
@@ -1746,6 +1854,12 @@
       <c r="H23" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="I23">
+        <v>75</v>
+      </c>
+      <c r="J23">
+        <v>16000</v>
+      </c>
       <c r="K23" s="1">
         <v>70</v>
       </c>
@@ -1781,6 +1895,12 @@
       <c r="H24" s="7" t="s">
         <v>112</v>
       </c>
+      <c r="I24">
+        <v>117</v>
+      </c>
+      <c r="J24">
+        <v>28000</v>
+      </c>
       <c r="K24" s="1">
         <v>147</v>
       </c>
@@ -1815,6 +1935,12 @@
       </c>
       <c r="H25" s="7" t="s">
         <v>112</v>
+      </c>
+      <c r="I25">
+        <v>50</v>
+      </c>
+      <c r="J25">
+        <v>15000</v>
       </c>
       <c r="K25" s="1">
         <v>90</v>

</xml_diff>

<commit_message>
Before Merge Main Into Branch
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsp1\Documents\GitHub\The-Cool-Guys\UnderChoices\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F386EC-6F15-44FE-AD4A-A239948CFC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445AEDB0-2B99-49B9-BBAC-75894154FDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="274">
   <si>
     <t>Post Number (Integer)</t>
   </si>
@@ -237,9 +237,6 @@
     <t>How Did This Anestheologist Work for 10 Years With No Training?</t>
   </si>
   <si>
-    <t>Anime Weebs Create Sword Art Online IRL</t>
-  </si>
-  <si>
     <t>Why Did Die A Hard Adrenaline Junkie Jump Without Her Parachute?</t>
   </si>
   <si>
@@ -838,6 +835,18 @@
   </si>
   <si>
     <t>Governments Repeated Attempts for Financial Trade Met with Harsh Rejection</t>
+  </si>
+  <si>
+    <t>Anime Enthusiasts Create Sword Art Online IRL</t>
+  </si>
+  <si>
+    <t>Government Forced to Raise Taxes</t>
+  </si>
+  <si>
+    <t>Arms on Sale!?! Arms Dealers Open Up to All During Civil Conflict!</t>
+  </si>
+  <si>
+    <t>Kids Forced Into Battle!!! Children now Expected to Carry Arms For Safety!</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L150" sqref="L150"/>
+    <sheetView tabSelected="1" topLeftCell="C118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L154" sqref="L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1354,7 @@
         <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1365,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>20</v>
@@ -1386,7 +1395,7 @@
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1406,13 +1415,13 @@
         <v>24</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="I4">
         <v>50</v>
@@ -1427,7 +1436,7 @@
         <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1447,13 +1456,13 @@
         <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K5" s="1">
         <v>75</v>
@@ -1462,7 +1471,7 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1482,13 +1491,13 @@
         <v>26</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K6" s="1">
         <v>121</v>
@@ -1497,7 +1506,7 @@
         <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1517,19 +1526,19 @@
         <v>26</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K7" s="1">
         <v>131</v>
       </c>
       <c r="L7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1549,19 +1558,19 @@
         <v>19</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K8" s="1">
         <v>98</v>
       </c>
       <c r="L8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1581,19 +1590,19 @@
         <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K9" s="1">
         <v>132</v>
       </c>
       <c r="L9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1616,16 +1625,16 @@
         <v>25</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K10" s="1">
         <v>149</v>
       </c>
       <c r="L10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1648,16 +1657,16 @@
         <v>25</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K11" s="1">
         <v>89</v>
       </c>
       <c r="L11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1677,19 +1686,19 @@
         <v>26</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="K12" s="1">
         <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1709,19 +1718,19 @@
         <v>26</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K13" s="1">
         <v>50</v>
       </c>
       <c r="L13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1741,13 +1750,13 @@
         <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K14" s="1">
         <v>134</v>
@@ -1756,7 +1765,7 @@
         <v>45</v>
       </c>
       <c r="M14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1776,13 +1785,13 @@
         <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K15" s="1">
         <v>78</v>
@@ -1791,7 +1800,7 @@
         <v>46</v>
       </c>
       <c r="M15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1811,19 +1820,19 @@
         <v>24</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K16" s="1">
         <v>145</v>
       </c>
       <c r="L16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1843,13 +1852,13 @@
         <v>24</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K17" s="1">
         <v>82</v>
@@ -1858,7 +1867,7 @@
         <v>48</v>
       </c>
       <c r="M17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1878,19 +1887,19 @@
         <v>26</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K18" s="1">
         <v>175</v>
       </c>
       <c r="L18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1910,19 +1919,19 @@
         <v>26</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K19" s="1">
         <v>91</v>
       </c>
       <c r="L19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1942,13 +1951,13 @@
         <v>19</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K20" s="1">
         <v>150</v>
@@ -1957,7 +1966,7 @@
         <v>50</v>
       </c>
       <c r="M20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1977,13 +1986,13 @@
         <v>19</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K21" s="1">
         <v>110</v>
@@ -1992,7 +2001,7 @@
         <v>51</v>
       </c>
       <c r="M21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2012,13 +2021,13 @@
         <v>24</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K22" s="1">
         <v>60</v>
@@ -2027,7 +2036,7 @@
         <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2047,13 +2056,13 @@
         <v>24</v>
       </c>
       <c r="F23" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K23" s="1">
         <v>70</v>
@@ -2062,7 +2071,7 @@
         <v>53</v>
       </c>
       <c r="M23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2082,13 +2091,13 @@
         <v>26</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K24" s="1">
         <v>147</v>
@@ -2097,7 +2106,7 @@
         <v>54</v>
       </c>
       <c r="M24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2117,13 +2126,13 @@
         <v>26</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K25" s="1">
         <v>90</v>
@@ -2132,7 +2141,7 @@
         <v>55</v>
       </c>
       <c r="M25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2164,10 +2173,10 @@
         <v>100</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2187,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
@@ -2199,10 +2208,10 @@
         <v>156</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2222,22 +2231,22 @@
         <v>24</v>
       </c>
       <c r="F28" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K28" s="1">
         <v>80</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2257,13 +2266,13 @@
         <v>24</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K29" s="1">
         <v>75</v>
@@ -2272,7 +2281,7 @@
         <v>56</v>
       </c>
       <c r="M29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2292,13 +2301,13 @@
         <v>26</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K30" s="1">
         <v>121</v>
@@ -2307,7 +2316,7 @@
         <v>57</v>
       </c>
       <c r="M30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2327,22 +2336,22 @@
         <v>26</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K31" s="1">
         <v>131</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2362,13 +2371,13 @@
         <v>19</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K32" s="1">
         <v>98</v>
@@ -2377,7 +2386,7 @@
         <v>58</v>
       </c>
       <c r="M32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2397,13 +2406,13 @@
         <v>19</v>
       </c>
       <c r="F33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K33" s="1">
         <v>132</v>
@@ -2412,7 +2421,7 @@
         <v>59</v>
       </c>
       <c r="M33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2435,10 +2444,10 @@
         <v>25</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K34" s="1">
         <v>149</v>
@@ -2447,7 +2456,7 @@
         <v>60</v>
       </c>
       <c r="M34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2470,10 +2479,10 @@
         <v>25</v>
       </c>
       <c r="G35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K35" s="1">
         <v>89</v>
@@ -2482,7 +2491,7 @@
         <v>61</v>
       </c>
       <c r="M35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2502,13 +2511,13 @@
         <v>26</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="H36" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K36" s="1">
         <v>69</v>
@@ -2517,7 +2526,7 @@
         <v>62</v>
       </c>
       <c r="M36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2537,13 +2546,13 @@
         <v>26</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K37" s="1">
         <v>50</v>
@@ -2552,7 +2561,7 @@
         <v>63</v>
       </c>
       <c r="M37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2572,13 +2581,13 @@
         <v>19</v>
       </c>
       <c r="F38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="H38" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K38" s="1">
         <v>134</v>
@@ -2587,7 +2596,7 @@
         <v>64</v>
       </c>
       <c r="M38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2607,13 +2616,13 @@
         <v>19</v>
       </c>
       <c r="F39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K39" s="1">
         <v>78</v>
@@ -2622,7 +2631,7 @@
         <v>65</v>
       </c>
       <c r="M39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2642,13 +2651,13 @@
         <v>24</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K40" s="1">
         <v>145</v>
@@ -2657,7 +2666,7 @@
         <v>66</v>
       </c>
       <c r="M40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2677,13 +2686,13 @@
         <v>24</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K41" s="1">
         <v>82</v>
@@ -2692,7 +2701,7 @@
         <v>67</v>
       </c>
       <c r="M41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2712,13 +2721,13 @@
         <v>26</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K42" s="1">
         <v>175</v>
@@ -2727,7 +2736,7 @@
         <v>68</v>
       </c>
       <c r="M42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2747,13 +2756,13 @@
         <v>26</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K43" s="1">
         <v>91</v>
@@ -2762,7 +2771,7 @@
         <v>69</v>
       </c>
       <c r="M43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2782,22 +2791,22 @@
         <v>19</v>
       </c>
       <c r="F44" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="H44" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K44" s="1">
         <v>150</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>70</v>
+        <v>270</v>
       </c>
       <c r="M44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2817,22 +2826,22 @@
         <v>19</v>
       </c>
       <c r="F45" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="H45" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K45" s="1">
         <v>110</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2852,22 +2861,22 @@
         <v>24</v>
       </c>
       <c r="F46" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="H46" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K46" s="1">
         <v>60</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2887,22 +2896,22 @@
         <v>24</v>
       </c>
       <c r="F47" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K47" s="1">
         <v>70</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2922,22 +2931,22 @@
         <v>26</v>
       </c>
       <c r="F48" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="H48" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K48" s="1">
         <v>147</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2957,22 +2966,22 @@
         <v>26</v>
       </c>
       <c r="F49" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="H49" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K49" s="1">
         <v>90</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3004,10 +3013,10 @@
         <v>100</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3027,7 +3036,7 @@
         <v>19</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G51" t="s">
         <v>20</v>
@@ -3039,7 +3048,7 @@
         <v>156</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3059,19 +3068,19 @@
         <v>24</v>
       </c>
       <c r="F52" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="H52" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K52" s="1">
         <v>80</v>
       </c>
       <c r="L52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3091,19 +3100,19 @@
         <v>24</v>
       </c>
       <c r="F53" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="H53" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K53" s="1">
         <v>75</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3123,19 +3132,19 @@
         <v>26</v>
       </c>
       <c r="F54" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="H54" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K54" s="1">
         <v>121</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3155,19 +3164,19 @@
         <v>26</v>
       </c>
       <c r="F55" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K55" s="1">
         <v>131</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3187,19 +3196,19 @@
         <v>19</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K56" s="1">
         <v>98</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3219,19 +3228,19 @@
         <v>19</v>
       </c>
       <c r="F57" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K57" s="1">
         <v>132</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3254,16 +3263,16 @@
         <v>25</v>
       </c>
       <c r="G58" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H58" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K58" s="1">
         <v>149</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3286,10 +3295,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H59" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K59" s="1">
         <v>89</v>
@@ -3298,7 +3307,7 @@
         <v>41</v>
       </c>
       <c r="M59" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3318,19 +3327,19 @@
         <v>26</v>
       </c>
       <c r="F60" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="H60" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K60" s="1">
         <v>69</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3350,19 +3359,19 @@
         <v>26</v>
       </c>
       <c r="F61" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G61" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="H61" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="K61" s="1">
         <v>50</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3382,19 +3391,19 @@
         <v>19</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G62" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="H62" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K62" s="1">
         <v>134</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3414,19 +3423,19 @@
         <v>19</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="H63" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K63" s="1">
         <v>78</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3446,19 +3455,19 @@
         <v>24</v>
       </c>
       <c r="F64" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G64" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="H64" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H64" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K64" s="1">
         <v>145</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3478,19 +3487,19 @@
         <v>24</v>
       </c>
       <c r="F65" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G65" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K65" s="1">
         <v>82</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3510,19 +3519,19 @@
         <v>26</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K66" s="1">
         <v>175</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3542,19 +3551,19 @@
         <v>26</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K67" s="1">
         <v>91</v>
       </c>
       <c r="L67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3574,19 +3583,19 @@
         <v>19</v>
       </c>
       <c r="F68" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G68" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="H68" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K68" s="1">
         <v>150</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3606,19 +3615,19 @@
         <v>19</v>
       </c>
       <c r="F69" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G69" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K69" s="1">
         <v>110</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3638,19 +3647,19 @@
         <v>24</v>
       </c>
       <c r="F70" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G70" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="H70" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K70" s="1">
         <v>60</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3670,19 +3679,19 @@
         <v>24</v>
       </c>
       <c r="F71" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G71" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K71" s="1">
         <v>70</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3702,19 +3711,19 @@
         <v>26</v>
       </c>
       <c r="F72" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G72" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="H72" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K72" s="1">
         <v>147</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3734,19 +3743,19 @@
         <v>26</v>
       </c>
       <c r="F73" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G73" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="7" t="s">
+      <c r="H73" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K73" s="1">
         <v>90</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3778,7 +3787,7 @@
         <v>100</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3798,7 +3807,7 @@
         <v>19</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G75" t="s">
         <v>20</v>
@@ -3810,7 +3819,7 @@
         <v>156</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3830,19 +3839,19 @@
         <v>24</v>
       </c>
       <c r="F76" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G76" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G76" s="4" t="s">
+      <c r="H76" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K76" s="1">
         <v>80</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3862,19 +3871,19 @@
         <v>24</v>
       </c>
       <c r="F77" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G77" s="4" t="s">
+      <c r="H77" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K77" s="1">
         <v>75</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3894,19 +3903,19 @@
         <v>26</v>
       </c>
       <c r="F78" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G78" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="H78" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H78" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K78" s="1">
         <v>121</v>
       </c>
       <c r="L78" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3926,19 +3935,19 @@
         <v>26</v>
       </c>
       <c r="F79" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G79" s="4" t="s">
+      <c r="H79" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K79" s="1">
         <v>131</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -3958,19 +3967,19 @@
         <v>19</v>
       </c>
       <c r="F80" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G80" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G80" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K80" s="1">
         <v>98</v>
       </c>
       <c r="L80" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -3990,19 +3999,19 @@
         <v>19</v>
       </c>
       <c r="F81" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G81" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G81" s="7" t="s">
+      <c r="H81" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K81" s="1">
         <v>132</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4025,16 +4034,16 @@
         <v>25</v>
       </c>
       <c r="G82" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K82" s="1">
         <v>149</v>
       </c>
       <c r="L82" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4057,10 +4066,10 @@
         <v>25</v>
       </c>
       <c r="G83" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H83" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K83" s="1">
         <v>89</v>
@@ -4069,7 +4078,7 @@
         <v>42</v>
       </c>
       <c r="M83" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4089,19 +4098,19 @@
         <v>26</v>
       </c>
       <c r="F84" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G84" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G84" s="7" t="s">
+      <c r="H84" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H84" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K84" s="1">
         <v>69</v>
       </c>
       <c r="L84" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4121,19 +4130,19 @@
         <v>26</v>
       </c>
       <c r="F85" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G85" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G85" s="7" t="s">
+      <c r="H85" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K85" s="1">
         <v>50</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4153,19 +4162,19 @@
         <v>19</v>
       </c>
       <c r="F86" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G86" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G86" s="7" t="s">
+      <c r="H86" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H86" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K86" s="1">
         <v>134</v>
       </c>
       <c r="L86" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4185,19 +4194,19 @@
         <v>19</v>
       </c>
       <c r="F87" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G87" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G87" s="7" t="s">
+      <c r="H87" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H87" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K87" s="1">
         <v>78</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4217,19 +4226,19 @@
         <v>24</v>
       </c>
       <c r="F88" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G88" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G88" s="7" t="s">
+      <c r="H88" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H88" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K88" s="1">
         <v>145</v>
       </c>
       <c r="L88" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4249,19 +4258,19 @@
         <v>24</v>
       </c>
       <c r="F89" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G89" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G89" s="7" t="s">
+      <c r="H89" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H89" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K89" s="1">
         <v>82</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4281,19 +4290,19 @@
         <v>26</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K90" s="1">
         <v>175</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4313,19 +4322,19 @@
         <v>26</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K91" s="1">
         <v>91</v>
       </c>
       <c r="L91" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4345,19 +4354,19 @@
         <v>19</v>
       </c>
       <c r="F92" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G92" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G92" s="7" t="s">
+      <c r="H92" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K92" s="1">
         <v>150</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4377,19 +4386,19 @@
         <v>19</v>
       </c>
       <c r="F93" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G93" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G93" s="7" t="s">
+      <c r="H93" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H93" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K93" s="1">
         <v>110</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4409,19 +4418,19 @@
         <v>24</v>
       </c>
       <c r="F94" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G94" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G94" s="7" t="s">
+      <c r="H94" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H94" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K94" s="1">
         <v>60</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4441,19 +4450,19 @@
         <v>24</v>
       </c>
       <c r="F95" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G95" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G95" s="7" t="s">
+      <c r="H95" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H95" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K95" s="1">
         <v>70</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4473,19 +4482,19 @@
         <v>26</v>
       </c>
       <c r="F96" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G96" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G96" s="7" t="s">
+      <c r="H96" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H96" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K96" s="1">
         <v>147</v>
       </c>
       <c r="L96" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4505,19 +4514,19 @@
         <v>26</v>
       </c>
       <c r="F97" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G97" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G97" s="7" t="s">
+      <c r="H97" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K97" s="1">
         <v>90</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4549,7 +4558,7 @@
         <v>100</v>
       </c>
       <c r="L98" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4569,7 +4578,7 @@
         <v>19</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G99" t="s">
         <v>20</v>
@@ -4581,7 +4590,7 @@
         <v>156</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4601,19 +4610,19 @@
         <v>24</v>
       </c>
       <c r="F100" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G100" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G100" s="4" t="s">
+      <c r="H100" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H100" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K100" s="1">
         <v>80</v>
       </c>
       <c r="L100" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4633,19 +4642,19 @@
         <v>24</v>
       </c>
       <c r="F101" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G101" s="4" t="s">
+      <c r="H101" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H101" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K101" s="1">
         <v>75</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4665,19 +4674,19 @@
         <v>26</v>
       </c>
       <c r="F102" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G102" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G102" s="4" t="s">
+      <c r="H102" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K102" s="1">
         <v>121</v>
       </c>
       <c r="L102" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4697,19 +4706,19 @@
         <v>26</v>
       </c>
       <c r="F103" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G103" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G103" s="4" t="s">
+      <c r="H103" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H103" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K103" s="1">
         <v>131</v>
       </c>
       <c r="L103" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4729,13 +4738,13 @@
         <v>19</v>
       </c>
       <c r="F104" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G104" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G104" s="7" t="s">
+      <c r="H104" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K104" s="1">
         <v>98</v>
@@ -4744,7 +4753,7 @@
         <v>39</v>
       </c>
       <c r="M104" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4764,19 +4773,19 @@
         <v>19</v>
       </c>
       <c r="F105" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G105" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G105" s="7" t="s">
+      <c r="H105" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K105" s="1">
         <v>132</v>
       </c>
       <c r="L105" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4799,10 +4808,10 @@
         <v>25</v>
       </c>
       <c r="G106" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H106" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H106" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K106" s="1">
         <v>149</v>
@@ -4811,7 +4820,7 @@
         <v>47</v>
       </c>
       <c r="M106" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4834,16 +4843,16 @@
         <v>25</v>
       </c>
       <c r="G107" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H107" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H107" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K107" s="1">
         <v>89</v>
       </c>
       <c r="L107" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4863,13 +4872,13 @@
         <v>26</v>
       </c>
       <c r="F108" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G108" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G108" s="7" t="s">
+      <c r="H108" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H108" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K108" s="1">
         <v>69</v>
@@ -4878,7 +4887,7 @@
         <v>43</v>
       </c>
       <c r="M108" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4898,19 +4907,19 @@
         <v>26</v>
       </c>
       <c r="F109" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G109" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G109" s="7" t="s">
+      <c r="H109" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H109" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K109" s="1">
         <v>50</v>
       </c>
       <c r="L109" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -4930,19 +4939,19 @@
         <v>19</v>
       </c>
       <c r="F110" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G110" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G110" s="7" t="s">
+      <c r="H110" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H110" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K110" s="1">
         <v>134</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -4962,19 +4971,19 @@
         <v>19</v>
       </c>
       <c r="F111" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G111" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G111" s="7" t="s">
+      <c r="H111" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H111" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K111" s="1">
         <v>78</v>
       </c>
       <c r="L111" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -4994,19 +5003,19 @@
         <v>24</v>
       </c>
       <c r="F112" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G112" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G112" s="7" t="s">
+      <c r="H112" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K112" s="1">
         <v>145</v>
       </c>
       <c r="L112" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5026,19 +5035,19 @@
         <v>24</v>
       </c>
       <c r="F113" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G113" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G113" s="7" t="s">
+      <c r="H113" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H113" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K113" s="1">
         <v>82</v>
       </c>
       <c r="L113" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5058,13 +5067,13 @@
         <v>26</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G114" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K114" s="1">
         <v>175</v>
@@ -5073,7 +5082,7 @@
         <v>49</v>
       </c>
       <c r="M114" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5093,19 +5102,19 @@
         <v>26</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K115" s="1">
         <v>91</v>
       </c>
       <c r="L115" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5125,19 +5134,19 @@
         <v>19</v>
       </c>
       <c r="F116" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G116" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G116" s="7" t="s">
+      <c r="H116" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H116" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K116" s="1">
         <v>150</v>
       </c>
       <c r="L116" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5157,19 +5166,19 @@
         <v>19</v>
       </c>
       <c r="F117" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G117" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G117" s="7" t="s">
+      <c r="H117" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H117" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K117" s="1">
         <v>110</v>
       </c>
       <c r="L117" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5189,19 +5198,19 @@
         <v>24</v>
       </c>
       <c r="F118" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G118" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G118" s="7" t="s">
+      <c r="H118" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K118" s="1">
         <v>60</v>
       </c>
       <c r="L118" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5221,19 +5230,19 @@
         <v>24</v>
       </c>
       <c r="F119" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G119" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G119" s="7" t="s">
+      <c r="H119" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K119" s="1">
         <v>70</v>
       </c>
       <c r="L119" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5253,19 +5262,19 @@
         <v>26</v>
       </c>
       <c r="F120" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G120" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G120" s="7" t="s">
+      <c r="H120" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H120" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K120" s="1">
         <v>147</v>
       </c>
       <c r="L120" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5285,19 +5294,19 @@
         <v>26</v>
       </c>
       <c r="F121" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G121" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G121" s="7" t="s">
+      <c r="H121" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K121" s="1">
         <v>90</v>
       </c>
       <c r="L121" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5329,7 +5338,7 @@
         <v>100</v>
       </c>
       <c r="L122" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5349,7 +5358,7 @@
         <v>19</v>
       </c>
       <c r="F123" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G123" t="s">
         <v>20</v>
@@ -5361,7 +5370,7 @@
         <v>156</v>
       </c>
       <c r="L123" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5381,19 +5390,19 @@
         <v>24</v>
       </c>
       <c r="F124" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G124" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G124" s="4" t="s">
+      <c r="H124" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H124" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K124" s="1">
         <v>80</v>
       </c>
       <c r="L124" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5413,19 +5422,19 @@
         <v>24</v>
       </c>
       <c r="F125" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G125" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G125" s="4" t="s">
+      <c r="H125" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H125" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K125" s="1">
         <v>75</v>
       </c>
       <c r="L125" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5445,19 +5454,19 @@
         <v>26</v>
       </c>
       <c r="F126" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G126" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G126" s="4" t="s">
+      <c r="H126" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H126" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K126" s="1">
         <v>121</v>
       </c>
       <c r="L126" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5477,19 +5486,19 @@
         <v>26</v>
       </c>
       <c r="F127" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G127" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G127" s="4" t="s">
+      <c r="H127" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H127" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K127" s="1">
         <v>131</v>
       </c>
       <c r="L127" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5509,19 +5518,19 @@
         <v>19</v>
       </c>
       <c r="F128" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G128" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G128" s="7" t="s">
+      <c r="H128" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H128" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K128" s="1">
         <v>98</v>
       </c>
       <c r="L128" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5541,19 +5550,19 @@
         <v>19</v>
       </c>
       <c r="F129" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G129" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G129" s="7" t="s">
+      <c r="H129" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H129" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K129" s="1">
         <v>132</v>
       </c>
       <c r="L129" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5576,16 +5585,16 @@
         <v>25</v>
       </c>
       <c r="G130" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H130" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H130" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K130" s="1">
         <v>149</v>
       </c>
       <c r="L130" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5608,16 +5617,16 @@
         <v>25</v>
       </c>
       <c r="G131" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H131" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H131" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K131" s="1">
         <v>89</v>
       </c>
       <c r="L131" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5637,13 +5646,13 @@
         <v>26</v>
       </c>
       <c r="F132" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G132" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G132" s="7" t="s">
+      <c r="H132" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K132" s="1">
         <v>69</v>
@@ -5652,7 +5661,7 @@
         <v>38</v>
       </c>
       <c r="M132" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5672,19 +5681,19 @@
         <v>26</v>
       </c>
       <c r="F133" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G133" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G133" s="7" t="s">
+      <c r="H133" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K133" s="1">
         <v>50</v>
       </c>
       <c r="L133" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5704,19 +5713,19 @@
         <v>19</v>
       </c>
       <c r="F134" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G134" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G134" s="7" t="s">
+      <c r="H134" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H134" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K134" s="1">
         <v>134</v>
       </c>
       <c r="L134" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5736,19 +5745,19 @@
         <v>19</v>
       </c>
       <c r="F135" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G135" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G135" s="7" t="s">
+      <c r="H135" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H135" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K135" s="1">
         <v>78</v>
       </c>
       <c r="L135" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -5768,19 +5777,19 @@
         <v>24</v>
       </c>
       <c r="F136" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G136" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G136" s="7" t="s">
+      <c r="H136" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K136" s="1">
         <v>145</v>
       </c>
       <c r="L136" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -5800,19 +5809,19 @@
         <v>24</v>
       </c>
       <c r="F137" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G137" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G137" s="7" t="s">
+      <c r="H137" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K137" s="1">
         <v>82</v>
       </c>
       <c r="L137" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -5832,22 +5841,22 @@
         <v>26</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G138" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H138" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K138" s="1">
         <v>175</v>
       </c>
       <c r="L138" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M138" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -5867,19 +5876,19 @@
         <v>26</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G139" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K139" s="1">
         <v>91</v>
       </c>
       <c r="L139" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -5899,19 +5908,19 @@
         <v>19</v>
       </c>
       <c r="F140" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G140" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G140" s="7" t="s">
+      <c r="H140" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K140" s="1">
         <v>150</v>
       </c>
       <c r="L140" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -5931,19 +5940,19 @@
         <v>19</v>
       </c>
       <c r="F141" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G141" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G141" s="7" t="s">
+      <c r="H141" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H141" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K141" s="1">
         <v>110</v>
       </c>
       <c r="L141" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -5963,19 +5972,19 @@
         <v>24</v>
       </c>
       <c r="F142" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G142" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G142" s="7" t="s">
+      <c r="H142" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H142" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K142" s="1">
         <v>60</v>
       </c>
       <c r="L142" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -5995,19 +6004,19 @@
         <v>24</v>
       </c>
       <c r="F143" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G143" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G143" s="7" t="s">
+      <c r="H143" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H143" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K143" s="1">
         <v>70</v>
       </c>
       <c r="L143" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6027,19 +6036,19 @@
         <v>26</v>
       </c>
       <c r="F144" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G144" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G144" s="7" t="s">
+      <c r="H144" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H144" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K144" s="1">
         <v>147</v>
       </c>
       <c r="L144" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6059,19 +6068,19 @@
         <v>26</v>
       </c>
       <c r="F145" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G145" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G145" s="7" t="s">
+      <c r="H145" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H145" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K145" s="1">
         <v>90</v>
       </c>
       <c r="L145" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6103,7 +6112,7 @@
         <v>100</v>
       </c>
       <c r="L146" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6123,7 +6132,7 @@
         <v>19</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G147" t="s">
         <v>20</v>
@@ -6135,7 +6144,7 @@
         <v>156</v>
       </c>
       <c r="L147" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6155,19 +6164,19 @@
         <v>24</v>
       </c>
       <c r="F148" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G148" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G148" s="4" t="s">
+      <c r="H148" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H148" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K148" s="1">
         <v>80</v>
       </c>
       <c r="L148" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6187,19 +6196,19 @@
         <v>24</v>
       </c>
       <c r="F149" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G149" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G149" s="4" t="s">
+      <c r="H149" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H149" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K149" s="1">
         <v>75</v>
       </c>
       <c r="L149" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6219,19 +6228,19 @@
         <v>26</v>
       </c>
       <c r="F150" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G150" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G150" s="4" t="s">
+      <c r="H150" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H150" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K150" s="1">
         <v>121</v>
       </c>
       <c r="L150" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6251,18 +6260,20 @@
         <v>26</v>
       </c>
       <c r="F151" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G151" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G151" s="4" t="s">
+      <c r="H151" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H151" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K151" s="1">
         <v>131</v>
       </c>
-      <c r="L151" s="4"/>
+      <c r="L151" s="4" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
@@ -6281,18 +6292,20 @@
         <v>19</v>
       </c>
       <c r="F152" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G152" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G152" s="7" t="s">
+      <c r="H152" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H152" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K152" s="1">
         <v>98</v>
       </c>
-      <c r="L152" s="5"/>
+      <c r="L152" s="5" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
@@ -6311,13 +6324,13 @@
         <v>19</v>
       </c>
       <c r="F153" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G153" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G153" s="7" t="s">
+      <c r="H153" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H153" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K153" s="1">
         <v>132</v>
@@ -6326,7 +6339,7 @@
         <v>40</v>
       </c>
       <c r="M153" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6349,10 +6362,10 @@
         <v>25</v>
       </c>
       <c r="G154" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H154" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H154" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K154" s="1">
         <v>149</v>
@@ -6379,10 +6392,10 @@
         <v>25</v>
       </c>
       <c r="G155" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H155" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H155" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K155" s="1">
         <v>89</v>
@@ -6406,18 +6419,20 @@
         <v>26</v>
       </c>
       <c r="F156" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G156" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G156" s="7" t="s">
+      <c r="H156" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H156" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K156" s="1">
         <v>69</v>
       </c>
-      <c r="L156" s="5"/>
+      <c r="L156" s="5" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
@@ -6436,13 +6451,13 @@
         <v>26</v>
       </c>
       <c r="F157" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G157" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G157" s="7" t="s">
+      <c r="H157" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H157" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K157" s="1">
         <v>50</v>
@@ -6466,13 +6481,13 @@
         <v>19</v>
       </c>
       <c r="F158" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G158" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G158" s="7" t="s">
+      <c r="H158" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H158" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K158" s="1">
         <v>134</v>
@@ -6496,13 +6511,13 @@
         <v>19</v>
       </c>
       <c r="F159" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G159" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G159" s="7" t="s">
+      <c r="H159" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H159" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K159" s="1">
         <v>78</v>
@@ -6526,13 +6541,13 @@
         <v>24</v>
       </c>
       <c r="F160" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G160" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G160" s="7" t="s">
+      <c r="H160" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H160" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K160" s="1">
         <v>145</v>
@@ -6556,13 +6571,13 @@
         <v>24</v>
       </c>
       <c r="F161" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G161" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G161" s="7" t="s">
+      <c r="H161" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H161" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K161" s="1">
         <v>82</v>
@@ -6586,13 +6601,13 @@
         <v>26</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G162" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H162" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K162" s="1">
         <v>175</v>
@@ -6616,13 +6631,13 @@
         <v>26</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G163" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H163" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K163" s="1">
         <v>91</v>
@@ -6646,13 +6661,13 @@
         <v>19</v>
       </c>
       <c r="F164" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G164" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G164" s="7" t="s">
+      <c r="H164" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H164" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K164" s="1">
         <v>150</v>
@@ -6676,13 +6691,13 @@
         <v>19</v>
       </c>
       <c r="F165" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G165" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G165" s="7" t="s">
+      <c r="H165" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H165" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K165" s="1">
         <v>110</v>
@@ -6706,13 +6721,13 @@
         <v>24</v>
       </c>
       <c r="F166" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G166" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G166" s="7" t="s">
+      <c r="H166" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H166" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K166" s="1">
         <v>60</v>
@@ -6736,13 +6751,13 @@
         <v>24</v>
       </c>
       <c r="F167" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G167" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G167" s="7" t="s">
+      <c r="H167" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H167" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K167" s="1">
         <v>70</v>
@@ -6766,13 +6781,13 @@
         <v>26</v>
       </c>
       <c r="F168" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G168" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G168" s="7" t="s">
+      <c r="H168" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H168" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K168" s="1">
         <v>147</v>
@@ -6796,13 +6811,13 @@
         <v>26</v>
       </c>
       <c r="F169" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G169" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G169" s="7" t="s">
+      <c r="H169" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H169" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K169" s="1">
         <v>90</v>
@@ -6841,7 +6856,7 @@
         <v>23</v>
       </c>
       <c r="M170" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -6861,7 +6876,7 @@
         <v>19</v>
       </c>
       <c r="F171" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G171" t="s">
         <v>20</v>
@@ -6891,13 +6906,13 @@
         <v>24</v>
       </c>
       <c r="F172" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G172" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G172" s="4" t="s">
+      <c r="H172" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H172" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K172" s="1">
         <v>80</v>
@@ -6921,13 +6936,13 @@
         <v>24</v>
       </c>
       <c r="F173" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G173" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G173" s="4" t="s">
+      <c r="H173" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H173" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="K173" s="1">
         <v>75</v>
@@ -6951,13 +6966,13 @@
         <v>26</v>
       </c>
       <c r="F174" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G174" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G174" s="4" t="s">
+      <c r="H174" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H174" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K174" s="1">
         <v>121</v>
@@ -6981,13 +6996,13 @@
         <v>26</v>
       </c>
       <c r="F175" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G175" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G175" s="4" t="s">
+      <c r="H175" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H175" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="K175" s="1">
         <v>131</v>
@@ -7011,13 +7026,13 @@
         <v>19</v>
       </c>
       <c r="F176" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G176" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G176" s="7" t="s">
+      <c r="H176" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H176" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K176" s="1">
         <v>98</v>
@@ -7041,13 +7056,13 @@
         <v>19</v>
       </c>
       <c r="F177" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G177" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G177" s="7" t="s">
+      <c r="H177" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H177" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="K177" s="1">
         <v>132</v>
@@ -7074,10 +7089,10 @@
         <v>25</v>
       </c>
       <c r="G178" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H178" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K178" s="1">
         <v>149</v>
@@ -7104,10 +7119,10 @@
         <v>25</v>
       </c>
       <c r="G179" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H179" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="H179" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="K179" s="1">
         <v>89</v>
@@ -7131,13 +7146,13 @@
         <v>26</v>
       </c>
       <c r="F180" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G180" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G180" s="7" t="s">
+      <c r="H180" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H180" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K180" s="1">
         <v>69</v>
@@ -7146,7 +7161,7 @@
         <v>44</v>
       </c>
       <c r="M180" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -7166,13 +7181,13 @@
         <v>26</v>
       </c>
       <c r="F181" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G181" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G181" s="7" t="s">
+      <c r="H181" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H181" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="K181" s="1">
         <v>50</v>
@@ -7196,13 +7211,13 @@
         <v>19</v>
       </c>
       <c r="F182" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G182" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G182" s="7" t="s">
+      <c r="H182" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H182" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K182" s="1">
         <v>134</v>
@@ -7226,13 +7241,13 @@
         <v>19</v>
       </c>
       <c r="F183" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G183" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G183" s="7" t="s">
+      <c r="H183" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H183" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="K183" s="1">
         <v>78</v>
@@ -7256,13 +7271,13 @@
         <v>24</v>
       </c>
       <c r="F184" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G184" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G184" s="7" t="s">
+      <c r="H184" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H184" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K184" s="1">
         <v>145</v>
@@ -7286,13 +7301,13 @@
         <v>24</v>
       </c>
       <c r="F185" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G185" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G185" s="7" t="s">
+      <c r="H185" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H185" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="K185" s="1">
         <v>82</v>
@@ -7316,13 +7331,13 @@
         <v>26</v>
       </c>
       <c r="F186" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G186" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K186" s="1">
         <v>175</v>
@@ -7346,13 +7361,13 @@
         <v>26</v>
       </c>
       <c r="F187" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G187" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H187" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K187" s="1">
         <v>91</v>
@@ -7376,13 +7391,13 @@
         <v>19</v>
       </c>
       <c r="F188" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G188" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G188" s="7" t="s">
+      <c r="H188" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H188" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K188" s="1">
         <v>150</v>
@@ -7406,13 +7421,13 @@
         <v>19</v>
       </c>
       <c r="F189" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G189" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G189" s="7" t="s">
+      <c r="H189" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H189" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K189" s="1">
         <v>110</v>
@@ -7436,13 +7451,13 @@
         <v>24</v>
       </c>
       <c r="F190" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G190" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G190" s="7" t="s">
+      <c r="H190" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H190" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K190" s="1">
         <v>60</v>
@@ -7466,13 +7481,13 @@
         <v>24</v>
       </c>
       <c r="F191" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G191" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G191" s="7" t="s">
+      <c r="H191" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H191" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="K191" s="1">
         <v>70</v>
@@ -7496,13 +7511,13 @@
         <v>26</v>
       </c>
       <c r="F192" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G192" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G192" s="7" t="s">
+      <c r="H192" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H192" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K192" s="1">
         <v>147</v>
@@ -7526,13 +7541,13 @@
         <v>26</v>
       </c>
       <c r="F193" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G193" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G193" s="7" t="s">
+      <c r="H193" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="H193" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="K193" s="1">
         <v>90</v>

</xml_diff>

<commit_message>
Final set of images for post
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsp1\Documents\GitHub\The-Cool-Guys\UnderChoices\Source\Narrative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\Desktop\Computer Science\BGDS Yr-03 Semester 06_Design_Practice_04\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C2CFC0-33DB-4E7F-8C6E-C6C7480642A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04160AC5-8727-434D-9222-0EC6047FE1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1369,22 +1369,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L194" sqref="L194"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="50.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="18.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="29.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="8" width="18.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="27.5703125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="10" max="10" width="30.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="19" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7866,6 +7866,11 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="B1:K1048576" sheet="Sheet1"/>
+    </dataRefs>
+  </dataConsolidate>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Named file image strings as "media_post_#"
</commit_message>
<xml_diff>
--- a/Source/Narrative/Media Posts.xlsx
+++ b/Source/Narrative/Media Posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\Desktop\Computer Science\BGDS Yr-03 Semester 06_Design_Practice_04\Source\Narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04160AC5-8727-434D-9222-0EC6047FE1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2C7DC7-9CA4-45F2-98B1-59BBAD967B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="448">
   <si>
     <t>Post Number (Integer)</t>
   </si>
@@ -348,153 +348,6 @@
     <t>Messiah</t>
   </si>
   <si>
-    <t>media_post_0.jpg</t>
-  </si>
-  <si>
-    <t>media_post_3.jpg</t>
-  </si>
-  <si>
-    <t>media_post_4.jpg</t>
-  </si>
-  <si>
-    <t>media_post_5.jpg</t>
-  </si>
-  <si>
-    <t>media_post_6.jpg</t>
-  </si>
-  <si>
-    <t>media_post_7.jpg</t>
-  </si>
-  <si>
-    <t>media_post_8.jpg</t>
-  </si>
-  <si>
-    <t>media_post_9.jpg</t>
-  </si>
-  <si>
-    <t>media_post_10.jpg</t>
-  </si>
-  <si>
-    <t>media_post_11.jpg</t>
-  </si>
-  <si>
-    <t>media_post_12.jpg</t>
-  </si>
-  <si>
-    <t>media_post_13.jpg</t>
-  </si>
-  <si>
-    <t>media_post_14.jpg</t>
-  </si>
-  <si>
-    <t>media_post_15.jpg</t>
-  </si>
-  <si>
-    <t>media_post_16.jpg</t>
-  </si>
-  <si>
-    <t>media_post_17.jpg</t>
-  </si>
-  <si>
-    <t>media_post_18.jpg</t>
-  </si>
-  <si>
-    <t>media_post_19.jpg</t>
-  </si>
-  <si>
-    <t>media_post_20.jpg</t>
-  </si>
-  <si>
-    <t>media_post_21.jpg</t>
-  </si>
-  <si>
-    <t>media_post_22.jpg</t>
-  </si>
-  <si>
-    <t>media_post_23.jpg</t>
-  </si>
-  <si>
-    <t>media_post_24.jpg</t>
-  </si>
-  <si>
-    <t>media_post_25.jpg</t>
-  </si>
-  <si>
-    <t>media_post_26.jpg</t>
-  </si>
-  <si>
-    <t>media_post_27.jpg</t>
-  </si>
-  <si>
-    <t>media_post_28.jpg</t>
-  </si>
-  <si>
-    <t>media_post_29.jpg</t>
-  </si>
-  <si>
-    <t>media_post_30.jpg</t>
-  </si>
-  <si>
-    <t>media_post_31.jpg</t>
-  </si>
-  <si>
-    <t>media_post_32.jpg</t>
-  </si>
-  <si>
-    <t>media_post_33.jpg</t>
-  </si>
-  <si>
-    <t>media_post_34.jpg</t>
-  </si>
-  <si>
-    <t>media_post_35.jpg</t>
-  </si>
-  <si>
-    <t>media_post_36.jpg</t>
-  </si>
-  <si>
-    <t>media_post_37.jpg</t>
-  </si>
-  <si>
-    <t>media_post_38.jpg</t>
-  </si>
-  <si>
-    <t>media_post_39.jpg</t>
-  </si>
-  <si>
-    <t>media_post_40.jpg</t>
-  </si>
-  <si>
-    <t>media_post_41.jpg</t>
-  </si>
-  <si>
-    <t>media_post_42.jpg</t>
-  </si>
-  <si>
-    <t>media_post_43.jpg</t>
-  </si>
-  <si>
-    <t>media_post_44.jpg</t>
-  </si>
-  <si>
-    <t>media_post_45.jpg</t>
-  </si>
-  <si>
-    <t>media_post_46.jpg</t>
-  </si>
-  <si>
-    <t>media_post_47.jpg</t>
-  </si>
-  <si>
-    <t>media_post_48.jpg</t>
-  </si>
-  <si>
-    <t>media_post_1.jpg</t>
-  </si>
-  <si>
-    <t>media_post_2.jpg</t>
-  </si>
-  <si>
     <t>U.S.A.R. Declares Smile Day a New Holiday!</t>
   </si>
   <si>
@@ -940,13 +793,589 @@
   </si>
   <si>
     <t>Filha Outraged! Storms Out Of Congress In Face Of Protestors!</t>
+  </si>
+  <si>
+    <t>media_post_0</t>
+  </si>
+  <si>
+    <t>media_post_5</t>
+  </si>
+  <si>
+    <t>media_post_6</t>
+  </si>
+  <si>
+    <t>media_post_7</t>
+  </si>
+  <si>
+    <t>media_post_8</t>
+  </si>
+  <si>
+    <t>media_post_9</t>
+  </si>
+  <si>
+    <t>media_post_10</t>
+  </si>
+  <si>
+    <t>media_post_11</t>
+  </si>
+  <si>
+    <t>media_post_14</t>
+  </si>
+  <si>
+    <t>media_post_16</t>
+  </si>
+  <si>
+    <t>media_post_17</t>
+  </si>
+  <si>
+    <t>media_post_1</t>
+  </si>
+  <si>
+    <t>media_post_2</t>
+  </si>
+  <si>
+    <t>media_post_3</t>
+  </si>
+  <si>
+    <t>media_post_4</t>
+  </si>
+  <si>
+    <t>media_post_12</t>
+  </si>
+  <si>
+    <t>media_post_13</t>
+  </si>
+  <si>
+    <t>media_post_15</t>
+  </si>
+  <si>
+    <t>media_post_18</t>
+  </si>
+  <si>
+    <t>media_post_19</t>
+  </si>
+  <si>
+    <t>media_post_20</t>
+  </si>
+  <si>
+    <t>media_post_21</t>
+  </si>
+  <si>
+    <t>media_post_22</t>
+  </si>
+  <si>
+    <t>media_post_23</t>
+  </si>
+  <si>
+    <t>media_post_24</t>
+  </si>
+  <si>
+    <t>media_post_25</t>
+  </si>
+  <si>
+    <t>media_post_26</t>
+  </si>
+  <si>
+    <t>media_post_27</t>
+  </si>
+  <si>
+    <t>media_post_28</t>
+  </si>
+  <si>
+    <t>media_post_29</t>
+  </si>
+  <si>
+    <t>media_post_30</t>
+  </si>
+  <si>
+    <t>media_post_31</t>
+  </si>
+  <si>
+    <t>media_post_32</t>
+  </si>
+  <si>
+    <t>media_post_33</t>
+  </si>
+  <si>
+    <t>media_post_34</t>
+  </si>
+  <si>
+    <t>media_post_35</t>
+  </si>
+  <si>
+    <t>media_post_36</t>
+  </si>
+  <si>
+    <t>media_post_37</t>
+  </si>
+  <si>
+    <t>media_post_38</t>
+  </si>
+  <si>
+    <t>media_post_39</t>
+  </si>
+  <si>
+    <t>media_post_40</t>
+  </si>
+  <si>
+    <t>media_post_41</t>
+  </si>
+  <si>
+    <t>media_post_42</t>
+  </si>
+  <si>
+    <t>media_post_43</t>
+  </si>
+  <si>
+    <t>media_post_44</t>
+  </si>
+  <si>
+    <t>media_post_45</t>
+  </si>
+  <si>
+    <t>media_post_46</t>
+  </si>
+  <si>
+    <t>media_post_47</t>
+  </si>
+  <si>
+    <t>media_post_48</t>
+  </si>
+  <si>
+    <t>media_post_49</t>
+  </si>
+  <si>
+    <t>media_post_50</t>
+  </si>
+  <si>
+    <t>media_post_51</t>
+  </si>
+  <si>
+    <t>media_post_52</t>
+  </si>
+  <si>
+    <t>media_post_53</t>
+  </si>
+  <si>
+    <t>media_post_54</t>
+  </si>
+  <si>
+    <t>media_post_55</t>
+  </si>
+  <si>
+    <t>media_post_56</t>
+  </si>
+  <si>
+    <t>media_post_57</t>
+  </si>
+  <si>
+    <t>media_post_58</t>
+  </si>
+  <si>
+    <t>media_post_59</t>
+  </si>
+  <si>
+    <t>media_post_60</t>
+  </si>
+  <si>
+    <t>media_post_61</t>
+  </si>
+  <si>
+    <t>media_post_62</t>
+  </si>
+  <si>
+    <t>media_post_63</t>
+  </si>
+  <si>
+    <t>media_post_64</t>
+  </si>
+  <si>
+    <t>media_post_65</t>
+  </si>
+  <si>
+    <t>media_post_66</t>
+  </si>
+  <si>
+    <t>media_post_67</t>
+  </si>
+  <si>
+    <t>media_post_68</t>
+  </si>
+  <si>
+    <t>media_post_69</t>
+  </si>
+  <si>
+    <t>media_post_70</t>
+  </si>
+  <si>
+    <t>media_post_71</t>
+  </si>
+  <si>
+    <t>media_post_72</t>
+  </si>
+  <si>
+    <t>media_post_73</t>
+  </si>
+  <si>
+    <t>media_post_74</t>
+  </si>
+  <si>
+    <t>media_post_75</t>
+  </si>
+  <si>
+    <t>media_post_76</t>
+  </si>
+  <si>
+    <t>media_post_77</t>
+  </si>
+  <si>
+    <t>media_post_78</t>
+  </si>
+  <si>
+    <t>media_post_79</t>
+  </si>
+  <si>
+    <t>media_post_80</t>
+  </si>
+  <si>
+    <t>media_post_81</t>
+  </si>
+  <si>
+    <t>media_post_82</t>
+  </si>
+  <si>
+    <t>media_post_83</t>
+  </si>
+  <si>
+    <t>media_post_84</t>
+  </si>
+  <si>
+    <t>media_post_85</t>
+  </si>
+  <si>
+    <t>media_post_86</t>
+  </si>
+  <si>
+    <t>media_post_87</t>
+  </si>
+  <si>
+    <t>media_post_88</t>
+  </si>
+  <si>
+    <t>media_post_89</t>
+  </si>
+  <si>
+    <t>media_post_90</t>
+  </si>
+  <si>
+    <t>media_post_91</t>
+  </si>
+  <si>
+    <t>media_post_92</t>
+  </si>
+  <si>
+    <t>media_post_93</t>
+  </si>
+  <si>
+    <t>media_post_94</t>
+  </si>
+  <si>
+    <t>media_post_95</t>
+  </si>
+  <si>
+    <t>media_post_96</t>
+  </si>
+  <si>
+    <t>media_post_97</t>
+  </si>
+  <si>
+    <t>media_post_98</t>
+  </si>
+  <si>
+    <t>media_post_99</t>
+  </si>
+  <si>
+    <t>media_post_100</t>
+  </si>
+  <si>
+    <t>media_post_101</t>
+  </si>
+  <si>
+    <t>media_post_102</t>
+  </si>
+  <si>
+    <t>media_post_103</t>
+  </si>
+  <si>
+    <t>media_post_104</t>
+  </si>
+  <si>
+    <t>media_post_105</t>
+  </si>
+  <si>
+    <t>media_post_106</t>
+  </si>
+  <si>
+    <t>media_post_107</t>
+  </si>
+  <si>
+    <t>media_post_108</t>
+  </si>
+  <si>
+    <t>media_post_109</t>
+  </si>
+  <si>
+    <t>media_post_110</t>
+  </si>
+  <si>
+    <t>media_post_111</t>
+  </si>
+  <si>
+    <t>media_post_112</t>
+  </si>
+  <si>
+    <t>media_post_113</t>
+  </si>
+  <si>
+    <t>media_post_114</t>
+  </si>
+  <si>
+    <t>media_post_115</t>
+  </si>
+  <si>
+    <t>media_post_116</t>
+  </si>
+  <si>
+    <t>media_post_117</t>
+  </si>
+  <si>
+    <t>media_post_118</t>
+  </si>
+  <si>
+    <t>media_post_119</t>
+  </si>
+  <si>
+    <t>media_post_120</t>
+  </si>
+  <si>
+    <t>media_post_121</t>
+  </si>
+  <si>
+    <t>media_post_122</t>
+  </si>
+  <si>
+    <t>media_post_123</t>
+  </si>
+  <si>
+    <t>media_post_124</t>
+  </si>
+  <si>
+    <t>media_post_125</t>
+  </si>
+  <si>
+    <t>media_post_126</t>
+  </si>
+  <si>
+    <t>media_post_127</t>
+  </si>
+  <si>
+    <t>media_post_128</t>
+  </si>
+  <si>
+    <t>media_post_129</t>
+  </si>
+  <si>
+    <t>media_post_130</t>
+  </si>
+  <si>
+    <t>media_post_131</t>
+  </si>
+  <si>
+    <t>media_post_132</t>
+  </si>
+  <si>
+    <t>media_post_133</t>
+  </si>
+  <si>
+    <t>media_post_134</t>
+  </si>
+  <si>
+    <t>media_post_135</t>
+  </si>
+  <si>
+    <t>media_post_136</t>
+  </si>
+  <si>
+    <t>media_post_137</t>
+  </si>
+  <si>
+    <t>media_post_138</t>
+  </si>
+  <si>
+    <t>media_post_139</t>
+  </si>
+  <si>
+    <t>media_post_140</t>
+  </si>
+  <si>
+    <t>media_post_141</t>
+  </si>
+  <si>
+    <t>media_post_142</t>
+  </si>
+  <si>
+    <t>media_post_143</t>
+  </si>
+  <si>
+    <t>media_post_144</t>
+  </si>
+  <si>
+    <t>media_post_145</t>
+  </si>
+  <si>
+    <t>media_post_146</t>
+  </si>
+  <si>
+    <t>media_post_147</t>
+  </si>
+  <si>
+    <t>media_post_148</t>
+  </si>
+  <si>
+    <t>media_post_149</t>
+  </si>
+  <si>
+    <t>media_post_150</t>
+  </si>
+  <si>
+    <t>media_post_151</t>
+  </si>
+  <si>
+    <t>media_post_152</t>
+  </si>
+  <si>
+    <t>media_post_153</t>
+  </si>
+  <si>
+    <t>media_post_154</t>
+  </si>
+  <si>
+    <t>media_post_155</t>
+  </si>
+  <si>
+    <t>media_post_156</t>
+  </si>
+  <si>
+    <t>media_post_157</t>
+  </si>
+  <si>
+    <t>media_post_158</t>
+  </si>
+  <si>
+    <t>media_post_159</t>
+  </si>
+  <si>
+    <t>media_post_160</t>
+  </si>
+  <si>
+    <t>media_post_161</t>
+  </si>
+  <si>
+    <t>media_post_162</t>
+  </si>
+  <si>
+    <t>media_post_163</t>
+  </si>
+  <si>
+    <t>media_post_164</t>
+  </si>
+  <si>
+    <t>media_post_165</t>
+  </si>
+  <si>
+    <t>media_post_166</t>
+  </si>
+  <si>
+    <t>media_post_167</t>
+  </si>
+  <si>
+    <t>media_post_168</t>
+  </si>
+  <si>
+    <t>media_post_169</t>
+  </si>
+  <si>
+    <t>media_post_170</t>
+  </si>
+  <si>
+    <t>media_post_171</t>
+  </si>
+  <si>
+    <t>media_post_172</t>
+  </si>
+  <si>
+    <t>media_post_173</t>
+  </si>
+  <si>
+    <t>media_post_174</t>
+  </si>
+  <si>
+    <t>media_post_175</t>
+  </si>
+  <si>
+    <t>media_post_176</t>
+  </si>
+  <si>
+    <t>media_post_177</t>
+  </si>
+  <si>
+    <t>media_post_178</t>
+  </si>
+  <si>
+    <t>media_post_179</t>
+  </si>
+  <si>
+    <t>media_post_180</t>
+  </si>
+  <si>
+    <t>media_post_181</t>
+  </si>
+  <si>
+    <t>media_post_182</t>
+  </si>
+  <si>
+    <t>media_post_183</t>
+  </si>
+  <si>
+    <t>media_post_184</t>
+  </si>
+  <si>
+    <t>media_post_185</t>
+  </si>
+  <si>
+    <t>media_post_186</t>
+  </si>
+  <si>
+    <t>media_post_187</t>
+  </si>
+  <si>
+    <t>media_post_188</t>
+  </si>
+  <si>
+    <t>media_post_189</t>
+  </si>
+  <si>
+    <t>media_post_190</t>
+  </si>
+  <si>
+    <t>media_post_191</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,8 +1396,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -978,18 +1413,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FFDDEBF7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
@@ -1006,7 +1429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1016,9 +1439,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,22 +1789,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="50.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="18.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="5" max="5" width="29.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="6" max="8" width="18.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="27.5703125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="10" max="10" width="30.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="19" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="8" width="18.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1" outlineLevel="2"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="19" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1465,7 +1885,10 @@
         <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>156</v>
+        <v>107</v>
+      </c>
+      <c r="M2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1506,7 +1929,7 @@
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>154</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1547,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1588,7 +2011,7 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>108</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1629,7 +2052,7 @@
         <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>109</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1667,7 +2090,10 @@
         <v>131</v>
       </c>
       <c r="L7" t="s">
-        <v>157</v>
+        <v>108</v>
+      </c>
+      <c r="M7" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1705,7 +2131,10 @@
         <v>98</v>
       </c>
       <c r="L8" t="s">
-        <v>158</v>
+        <v>109</v>
+      </c>
+      <c r="M8" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1743,7 +2172,10 @@
         <v>132</v>
       </c>
       <c r="L9" t="s">
-        <v>159</v>
+        <v>110</v>
+      </c>
+      <c r="M9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1781,7 +2213,10 @@
         <v>149</v>
       </c>
       <c r="L10" t="s">
-        <v>160</v>
+        <v>111</v>
+      </c>
+      <c r="M10" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1819,7 +2254,10 @@
         <v>89</v>
       </c>
       <c r="L11" t="s">
-        <v>161</v>
+        <v>112</v>
+      </c>
+      <c r="M11" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1857,7 +2295,10 @@
         <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>280</v>
+        <v>231</v>
+      </c>
+      <c r="M12" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1895,7 +2336,10 @@
         <v>50</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>113</v>
+      </c>
+      <c r="M13" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1936,7 +2380,7 @@
         <v>45</v>
       </c>
       <c r="M14" t="s">
-        <v>117</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1977,7 +2421,7 @@
         <v>46</v>
       </c>
       <c r="M15" t="s">
-        <v>118</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2015,7 +2459,10 @@
         <v>145</v>
       </c>
       <c r="L16" t="s">
-        <v>163</v>
+        <v>114</v>
+      </c>
+      <c r="M16" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2056,7 +2503,7 @@
         <v>48</v>
       </c>
       <c r="M17" t="s">
-        <v>120</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2094,7 +2541,10 @@
         <v>175</v>
       </c>
       <c r="L18" t="s">
-        <v>164</v>
+        <v>115</v>
+      </c>
+      <c r="M18" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2132,7 +2582,10 @@
         <v>91</v>
       </c>
       <c r="L19" t="s">
-        <v>165</v>
+        <v>116</v>
+      </c>
+      <c r="M19" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2173,7 +2626,7 @@
         <v>50</v>
       </c>
       <c r="M20" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2214,7 +2667,7 @@
         <v>51</v>
       </c>
       <c r="M21" t="s">
-        <v>124</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2255,7 +2708,7 @@
         <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>125</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2296,7 +2749,7 @@
         <v>53</v>
       </c>
       <c r="M23" t="s">
-        <v>126</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2337,7 +2790,7 @@
         <v>54</v>
       </c>
       <c r="M24" t="s">
-        <v>127</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2378,7 +2831,7 @@
         <v>55</v>
       </c>
       <c r="M25" t="s">
-        <v>128</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2410,10 +2863,10 @@
         <v>100</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
       <c r="M26" t="s">
-        <v>129</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2445,10 +2898,10 @@
         <v>156</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="M27" t="s">
-        <v>130</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2480,10 +2933,10 @@
         <v>80</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="M28" t="s">
-        <v>131</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2518,7 +2971,7 @@
         <v>56</v>
       </c>
       <c r="M29" t="s">
-        <v>132</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2553,7 +3006,7 @@
         <v>57</v>
       </c>
       <c r="M30" t="s">
-        <v>133</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2585,10 +3038,10 @@
         <v>131</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="M31" t="s">
-        <v>134</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2623,7 +3076,7 @@
         <v>58</v>
       </c>
       <c r="M32" t="s">
-        <v>135</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2658,7 +3111,7 @@
         <v>59</v>
       </c>
       <c r="M33" t="s">
-        <v>136</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2693,7 +3146,7 @@
         <v>60</v>
       </c>
       <c r="M34" t="s">
-        <v>137</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2728,7 +3181,7 @@
         <v>61</v>
       </c>
       <c r="M35" t="s">
-        <v>138</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2763,7 +3216,7 @@
         <v>62</v>
       </c>
       <c r="M36" t="s">
-        <v>139</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2798,7 +3251,7 @@
         <v>63</v>
       </c>
       <c r="M37" t="s">
-        <v>140</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2833,7 +3286,7 @@
         <v>64</v>
       </c>
       <c r="M38" t="s">
-        <v>141</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2868,7 +3321,7 @@
         <v>65</v>
       </c>
       <c r="M39" t="s">
-        <v>142</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2903,7 +3356,7 @@
         <v>66</v>
       </c>
       <c r="M40" t="s">
-        <v>143</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2938,7 +3391,7 @@
         <v>67</v>
       </c>
       <c r="M41" t="s">
-        <v>144</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2973,7 +3426,7 @@
         <v>68</v>
       </c>
       <c r="M42" t="s">
-        <v>145</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3008,7 +3461,7 @@
         <v>69</v>
       </c>
       <c r="M43" t="s">
-        <v>146</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3040,10 +3493,10 @@
         <v>150</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="M44" t="s">
-        <v>147</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3078,7 +3531,7 @@
         <v>74</v>
       </c>
       <c r="M45" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3113,7 +3566,7 @@
         <v>70</v>
       </c>
       <c r="M46" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3148,7 +3601,7 @@
         <v>71</v>
       </c>
       <c r="M47" t="s">
-        <v>150</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3183,7 +3636,7 @@
         <v>72</v>
       </c>
       <c r="M48" t="s">
-        <v>151</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3218,7 +3671,7 @@
         <v>73</v>
       </c>
       <c r="M49" t="s">
-        <v>152</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3250,10 +3703,10 @@
         <v>100</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>153</v>
+        <v>122</v>
+      </c>
+      <c r="M50" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3285,7 +3738,10 @@
         <v>156</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>172</v>
+        <v>123</v>
+      </c>
+      <c r="M51" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3317,7 +3773,10 @@
         <v>80</v>
       </c>
       <c r="L52" t="s">
-        <v>173</v>
+        <v>124</v>
+      </c>
+      <c r="M52" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3349,7 +3808,10 @@
         <v>75</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>174</v>
+        <v>125</v>
+      </c>
+      <c r="M53" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3381,7 +3843,10 @@
         <v>121</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>175</v>
+        <v>126</v>
+      </c>
+      <c r="M54" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3413,7 +3878,10 @@
         <v>131</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="M55" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3445,7 +3913,10 @@
         <v>98</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>177</v>
+        <v>128</v>
+      </c>
+      <c r="M56" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3477,7 +3948,10 @@
         <v>132</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>178</v>
+        <v>129</v>
+      </c>
+      <c r="M57" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3509,7 +3983,10 @@
         <v>149</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>179</v>
+        <v>130</v>
+      </c>
+      <c r="M58" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3540,11 +4017,11 @@
       <c r="K59" s="1">
         <v>89</v>
       </c>
-      <c r="L59" s="10" t="s">
+      <c r="L59" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M59" s="9" t="s">
-        <v>113</v>
+      <c r="M59" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3576,7 +4053,10 @@
         <v>69</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>180</v>
+        <v>131</v>
+      </c>
+      <c r="M60" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3608,7 +4088,10 @@
         <v>50</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>281</v>
+        <v>232</v>
+      </c>
+      <c r="M61" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3640,7 +4123,10 @@
         <v>134</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>181</v>
+        <v>132</v>
+      </c>
+      <c r="M62" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3672,7 +4158,10 @@
         <v>78</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>182</v>
+        <v>133</v>
+      </c>
+      <c r="M63" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3704,10 +4193,13 @@
         <v>145</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="M64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3736,10 +4228,13 @@
         <v>82</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="M65" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -3768,10 +4263,13 @@
         <v>175</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="M66" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3800,10 +4298,13 @@
         <v>91</v>
       </c>
       <c r="L67" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="M67" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -3832,10 +4333,13 @@
         <v>150</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="M68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -3864,10 +4368,13 @@
         <v>110</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="M69" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -3896,10 +4403,13 @@
         <v>60</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="M70" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3928,10 +4438,13 @@
         <v>70</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="M71" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -3960,10 +4473,13 @@
         <v>147</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="M72" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -3992,10 +4508,13 @@
         <v>90</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="M73" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -4024,10 +4543,13 @@
         <v>100</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="M74" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -4056,10 +4578,13 @@
         <v>156</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="M75" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -4088,10 +4613,13 @@
         <v>80</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="M76" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -4120,10 +4648,13 @@
         <v>75</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="M77" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -4152,10 +4683,13 @@
         <v>121</v>
       </c>
       <c r="L78" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="M78" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -4184,10 +4718,13 @@
         <v>131</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="M79" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -4215,8 +4752,11 @@
       <c r="K80" s="1">
         <v>98</v>
       </c>
-      <c r="L80" s="5" t="s">
-        <v>198</v>
+      <c r="L80" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="M80" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4247,8 +4787,11 @@
       <c r="K81" s="1">
         <v>132</v>
       </c>
-      <c r="L81" s="4" t="s">
-        <v>199</v>
+      <c r="L81" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="M81" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4279,8 +4822,11 @@
       <c r="K82" s="1">
         <v>149</v>
       </c>
-      <c r="L82" s="5" t="s">
-        <v>200</v>
+      <c r="L82" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="M82" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4311,11 +4857,11 @@
       <c r="K83" s="1">
         <v>89</v>
       </c>
-      <c r="L83" s="11" t="s">
+      <c r="L83" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M83" s="9" t="s">
-        <v>114</v>
+      <c r="M83" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4346,8 +4892,11 @@
       <c r="K84" s="1">
         <v>69</v>
       </c>
-      <c r="L84" s="5" t="s">
-        <v>201</v>
+      <c r="L84" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="M84" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4378,8 +4927,11 @@
       <c r="K85" s="1">
         <v>50</v>
       </c>
-      <c r="L85" s="4" t="s">
-        <v>202</v>
+      <c r="L85" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="M85" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4410,8 +4962,11 @@
       <c r="K86" s="1">
         <v>134</v>
       </c>
-      <c r="L86" s="5" t="s">
-        <v>203</v>
+      <c r="L86" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="M86" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4442,8 +4997,11 @@
       <c r="K87" s="1">
         <v>78</v>
       </c>
-      <c r="L87" s="4" t="s">
-        <v>204</v>
+      <c r="L87" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="M87" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4474,8 +5032,11 @@
       <c r="K88" s="1">
         <v>145</v>
       </c>
-      <c r="L88" s="5" t="s">
-        <v>205</v>
+      <c r="L88" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M88" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4506,8 +5067,11 @@
       <c r="K89" s="1">
         <v>82</v>
       </c>
-      <c r="L89" s="4" t="s">
-        <v>206</v>
+      <c r="L89" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="M89" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4538,8 +5102,11 @@
       <c r="K90" s="1">
         <v>175</v>
       </c>
-      <c r="L90" s="5" t="s">
-        <v>207</v>
+      <c r="L90" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="M90" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4570,8 +5137,11 @@
       <c r="K91" s="1">
         <v>91</v>
       </c>
-      <c r="L91" s="4" t="s">
-        <v>208</v>
+      <c r="L91" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M91" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4602,8 +5172,11 @@
       <c r="K92" s="1">
         <v>150</v>
       </c>
-      <c r="L92" s="5" t="s">
-        <v>209</v>
+      <c r="L92" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="M92" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4634,8 +5207,11 @@
       <c r="K93" s="1">
         <v>110</v>
       </c>
-      <c r="L93" s="4" t="s">
-        <v>210</v>
+      <c r="L93" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="M93" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4666,8 +5242,11 @@
       <c r="K94" s="1">
         <v>60</v>
       </c>
-      <c r="L94" s="5" t="s">
-        <v>211</v>
+      <c r="L94" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="M94" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4698,8 +5277,11 @@
       <c r="K95" s="1">
         <v>70</v>
       </c>
-      <c r="L95" s="4" t="s">
-        <v>212</v>
+      <c r="L95" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="M95" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4730,8 +5312,11 @@
       <c r="K96" s="1">
         <v>147</v>
       </c>
-      <c r="L96" s="5" t="s">
-        <v>213</v>
+      <c r="L96" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M96" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4762,8 +5347,11 @@
       <c r="K97" s="1">
         <v>90</v>
       </c>
-      <c r="L97" s="4" t="s">
-        <v>214</v>
+      <c r="L97" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="M97" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4794,8 +5382,11 @@
       <c r="K98" s="1">
         <v>100</v>
       </c>
-      <c r="L98" s="5" t="s">
-        <v>215</v>
+      <c r="L98" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="M98" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4826,8 +5417,11 @@
       <c r="K99" s="1">
         <v>156</v>
       </c>
-      <c r="L99" s="4" t="s">
-        <v>216</v>
+      <c r="L99" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="M99" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4858,8 +5452,11 @@
       <c r="K100" s="1">
         <v>80</v>
       </c>
-      <c r="L100" s="5" t="s">
-        <v>217</v>
+      <c r="L100" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M100" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4890,8 +5487,11 @@
       <c r="K101" s="1">
         <v>75</v>
       </c>
-      <c r="L101" s="4" t="s">
-        <v>218</v>
+      <c r="L101" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M101" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4922,8 +5522,11 @@
       <c r="K102" s="1">
         <v>121</v>
       </c>
-      <c r="L102" s="5" t="s">
-        <v>219</v>
+      <c r="L102" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="M102" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4954,8 +5557,11 @@
       <c r="K103" s="1">
         <v>131</v>
       </c>
-      <c r="L103" s="4" t="s">
-        <v>220</v>
+      <c r="L103" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="M103" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4986,11 +5592,11 @@
       <c r="K104" s="1">
         <v>98</v>
       </c>
-      <c r="L104" s="10" t="s">
+      <c r="L104" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M104" s="9" t="s">
-        <v>111</v>
+      <c r="M104" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -5021,8 +5627,11 @@
       <c r="K105" s="1">
         <v>132</v>
       </c>
-      <c r="L105" s="4" t="s">
-        <v>221</v>
+      <c r="L105" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M105" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -5053,11 +5662,11 @@
       <c r="K106" s="1">
         <v>149</v>
       </c>
-      <c r="L106" s="10" t="s">
+      <c r="L106" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="M106" s="9" t="s">
-        <v>119</v>
+      <c r="M106" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -5088,8 +5697,11 @@
       <c r="K107" s="1">
         <v>89</v>
       </c>
-      <c r="L107" s="4" t="s">
-        <v>222</v>
+      <c r="L107" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="M107" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -5120,11 +5732,11 @@
       <c r="K108" s="1">
         <v>69</v>
       </c>
-      <c r="L108" s="10" t="s">
+      <c r="L108" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M108" s="9" t="s">
-        <v>115</v>
+      <c r="M108" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -5155,8 +5767,11 @@
       <c r="K109" s="1">
         <v>50</v>
       </c>
-      <c r="L109" s="4" t="s">
-        <v>282</v>
+      <c r="L109" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="M109" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -5187,8 +5802,11 @@
       <c r="K110" s="1">
         <v>134</v>
       </c>
-      <c r="L110" s="5" t="s">
-        <v>223</v>
+      <c r="L110" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="M110" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -5219,8 +5837,11 @@
       <c r="K111" s="1">
         <v>78</v>
       </c>
-      <c r="L111" s="4" t="s">
-        <v>224</v>
+      <c r="L111" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="M111" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -5251,8 +5872,11 @@
       <c r="K112" s="1">
         <v>145</v>
       </c>
-      <c r="L112" s="5" t="s">
-        <v>225</v>
+      <c r="L112" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="M112" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5283,8 +5907,11 @@
       <c r="K113" s="1">
         <v>82</v>
       </c>
-      <c r="L113" s="4" t="s">
-        <v>226</v>
+      <c r="L113" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="M113" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5315,11 +5942,11 @@
       <c r="K114" s="1">
         <v>175</v>
       </c>
-      <c r="L114" s="11" t="s">
+      <c r="L114" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M114" s="9" t="s">
-        <v>122</v>
+      <c r="M114" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5350,8 +5977,11 @@
       <c r="K115" s="1">
         <v>91</v>
       </c>
-      <c r="L115" s="4" t="s">
-        <v>227</v>
+      <c r="L115" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="M115" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5382,8 +6012,11 @@
       <c r="K116" s="1">
         <v>150</v>
       </c>
-      <c r="L116" s="5" t="s">
-        <v>228</v>
+      <c r="L116" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="M116" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5414,8 +6047,11 @@
       <c r="K117" s="1">
         <v>110</v>
       </c>
-      <c r="L117" s="4" t="s">
-        <v>229</v>
+      <c r="L117" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="M117" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5446,8 +6082,11 @@
       <c r="K118" s="1">
         <v>60</v>
       </c>
-      <c r="L118" s="5" t="s">
-        <v>230</v>
+      <c r="L118" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M118" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5478,8 +6117,11 @@
       <c r="K119" s="1">
         <v>70</v>
       </c>
-      <c r="L119" s="4" t="s">
-        <v>231</v>
+      <c r="L119" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="M119" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5510,8 +6152,11 @@
       <c r="K120" s="1">
         <v>147</v>
       </c>
-      <c r="L120" s="5" t="s">
-        <v>232</v>
+      <c r="L120" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="M120" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5542,8 +6187,11 @@
       <c r="K121" s="1">
         <v>90</v>
       </c>
-      <c r="L121" s="4" t="s">
-        <v>233</v>
+      <c r="L121" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="M121" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5574,8 +6222,11 @@
       <c r="K122" s="1">
         <v>100</v>
       </c>
-      <c r="L122" s="5" t="s">
-        <v>234</v>
+      <c r="L122" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="M122" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5606,8 +6257,11 @@
       <c r="K123" s="1">
         <v>156</v>
       </c>
-      <c r="L123" t="s">
-        <v>235</v>
+      <c r="L123" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="M123" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5638,8 +6292,11 @@
       <c r="K124" s="1">
         <v>80</v>
       </c>
-      <c r="L124" s="5" t="s">
-        <v>236</v>
+      <c r="L124" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="M124" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5670,8 +6327,11 @@
       <c r="K125" s="1">
         <v>75</v>
       </c>
-      <c r="L125" s="4" t="s">
-        <v>237</v>
+      <c r="L125" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="M125" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5702,8 +6362,11 @@
       <c r="K126" s="1">
         <v>121</v>
       </c>
-      <c r="L126" s="5" t="s">
-        <v>238</v>
+      <c r="L126" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="M126" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5734,8 +6397,11 @@
       <c r="K127" s="1">
         <v>131</v>
       </c>
-      <c r="L127" s="4" t="s">
-        <v>239</v>
+      <c r="L127" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="M127" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5766,8 +6432,11 @@
       <c r="K128" s="1">
         <v>98</v>
       </c>
-      <c r="L128" s="5" t="s">
-        <v>240</v>
+      <c r="L128" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="M128" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5798,8 +6467,11 @@
       <c r="K129" s="1">
         <v>132</v>
       </c>
-      <c r="L129" s="4" t="s">
-        <v>241</v>
+      <c r="L129" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="M129" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5830,8 +6502,11 @@
       <c r="K130" s="1">
         <v>149</v>
       </c>
-      <c r="L130" s="5" t="s">
-        <v>242</v>
+      <c r="L130" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="M130" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5862,8 +6537,11 @@
       <c r="K131" s="1">
         <v>89</v>
       </c>
-      <c r="L131" s="4" t="s">
-        <v>243</v>
+      <c r="L131" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="M131" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5894,11 +6572,11 @@
       <c r="K132" s="1">
         <v>69</v>
       </c>
-      <c r="L132" s="11" t="s">
+      <c r="L132" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M132" s="9" t="s">
-        <v>110</v>
+      <c r="M132" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5929,8 +6607,11 @@
       <c r="K133" s="1">
         <v>50</v>
       </c>
-      <c r="L133" s="5" t="s">
-        <v>244</v>
+      <c r="L133" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="M133" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5961,8 +6642,11 @@
       <c r="K134" s="1">
         <v>134</v>
       </c>
-      <c r="L134" s="5" t="s">
-        <v>245</v>
+      <c r="L134" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="M134" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5993,8 +6677,11 @@
       <c r="K135" s="1">
         <v>78</v>
       </c>
-      <c r="L135" s="4" t="s">
-        <v>246</v>
+      <c r="L135" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M135" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -6025,8 +6712,11 @@
       <c r="K136" s="1">
         <v>145</v>
       </c>
-      <c r="L136" s="5" t="s">
-        <v>247</v>
+      <c r="L136" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="M136" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -6057,8 +6747,11 @@
       <c r="K137" s="1">
         <v>82</v>
       </c>
-      <c r="L137" s="4" t="s">
-        <v>248</v>
+      <c r="L137" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="M137" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -6089,11 +6782,11 @@
       <c r="K138" s="1">
         <v>175</v>
       </c>
-      <c r="L138" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="M138" s="9" t="s">
-        <v>121</v>
+      <c r="L138" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="M138" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -6124,8 +6817,11 @@
       <c r="K139" s="1">
         <v>91</v>
       </c>
-      <c r="L139" s="4" t="s">
-        <v>250</v>
+      <c r="L139" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="M139" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -6156,8 +6852,11 @@
       <c r="K140" s="1">
         <v>150</v>
       </c>
-      <c r="L140" s="5" t="s">
-        <v>251</v>
+      <c r="L140" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="M140" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -6188,8 +6887,11 @@
       <c r="K141" s="1">
         <v>110</v>
       </c>
-      <c r="L141" s="4" t="s">
-        <v>252</v>
+      <c r="L141" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="M141" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -6220,8 +6922,11 @@
       <c r="K142" s="1">
         <v>60</v>
       </c>
-      <c r="L142" s="5" t="s">
-        <v>253</v>
+      <c r="L142" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="M142" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -6252,8 +6957,11 @@
       <c r="K143" s="1">
         <v>70</v>
       </c>
-      <c r="L143" s="4" t="s">
-        <v>254</v>
+      <c r="L143" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="M143" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6284,8 +6992,11 @@
       <c r="K144" s="1">
         <v>147</v>
       </c>
-      <c r="L144" s="5" t="s">
-        <v>255</v>
+      <c r="L144" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="M144" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6316,8 +7027,11 @@
       <c r="K145" s="1">
         <v>90</v>
       </c>
-      <c r="L145" s="4" t="s">
-        <v>265</v>
+      <c r="L145" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M145" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6348,8 +7062,11 @@
       <c r="K146" s="1">
         <v>100</v>
       </c>
-      <c r="L146" s="4" t="s">
-        <v>256</v>
+      <c r="L146" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="M146" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6380,8 +7097,11 @@
       <c r="K147" s="1">
         <v>156</v>
       </c>
-      <c r="L147" s="4" t="s">
-        <v>257</v>
+      <c r="L147" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M147" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6412,8 +7132,11 @@
       <c r="K148" s="1">
         <v>80</v>
       </c>
-      <c r="L148" s="5" t="s">
-        <v>258</v>
+      <c r="L148" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="M148" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6444,8 +7167,11 @@
       <c r="K149" s="1">
         <v>75</v>
       </c>
-      <c r="L149" s="4" t="s">
-        <v>259</v>
+      <c r="L149" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="M149" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6476,8 +7202,11 @@
       <c r="K150" s="1">
         <v>121</v>
       </c>
-      <c r="L150" s="5" t="s">
-        <v>260</v>
+      <c r="L150" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="M150" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6508,8 +7237,11 @@
       <c r="K151" s="1">
         <v>131</v>
       </c>
-      <c r="L151" s="4" t="s">
-        <v>261</v>
+      <c r="L151" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="M151" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -6540,8 +7272,11 @@
       <c r="K152" s="1">
         <v>98</v>
       </c>
-      <c r="L152" s="5" t="s">
-        <v>262</v>
+      <c r="L152" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="M152" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -6572,11 +7307,11 @@
       <c r="K153" s="1">
         <v>132</v>
       </c>
-      <c r="L153" s="11" t="s">
+      <c r="L153" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M153" s="9" t="s">
-        <v>112</v>
+      <c r="M153" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6607,8 +7342,11 @@
       <c r="K154" s="1">
         <v>149</v>
       </c>
-      <c r="L154" s="5" t="s">
-        <v>263</v>
+      <c r="L154" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="M154" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -6639,8 +7377,11 @@
       <c r="K155" s="1">
         <v>89</v>
       </c>
-      <c r="L155" s="4" t="s">
-        <v>264</v>
+      <c r="L155" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="M155" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -6671,8 +7412,11 @@
       <c r="K156" s="1">
         <v>69</v>
       </c>
-      <c r="L156" s="5" t="s">
-        <v>266</v>
+      <c r="L156" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="M156" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -6703,8 +7447,11 @@
       <c r="K157" s="1">
         <v>50</v>
       </c>
-      <c r="L157" s="4" t="s">
-        <v>267</v>
+      <c r="L157" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="M157" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -6735,8 +7482,11 @@
       <c r="K158" s="1">
         <v>134</v>
       </c>
-      <c r="L158" s="5" t="s">
-        <v>268</v>
+      <c r="L158" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="M158" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -6767,8 +7517,11 @@
       <c r="K159" s="1">
         <v>78</v>
       </c>
-      <c r="L159" s="4" t="s">
-        <v>269</v>
+      <c r="L159" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="M159" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -6799,8 +7552,11 @@
       <c r="K160" s="1">
         <v>145</v>
       </c>
-      <c r="L160" s="5" t="s">
-        <v>270</v>
+      <c r="L160" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="M160" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -6831,8 +7587,11 @@
       <c r="K161" s="1">
         <v>82</v>
       </c>
-      <c r="L161" s="4" t="s">
-        <v>271</v>
+      <c r="L161" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="M161" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -6863,8 +7622,11 @@
       <c r="K162" s="1">
         <v>175</v>
       </c>
-      <c r="L162" s="5" t="s">
-        <v>272</v>
+      <c r="L162" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="M162" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -6895,8 +7657,11 @@
       <c r="K163" s="1">
         <v>91</v>
       </c>
-      <c r="L163" s="4" t="s">
-        <v>273</v>
+      <c r="L163" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="M163" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -6927,8 +7692,11 @@
       <c r="K164" s="1">
         <v>150</v>
       </c>
-      <c r="L164" s="5" t="s">
-        <v>275</v>
+      <c r="L164" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="M164" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -6959,8 +7727,11 @@
       <c r="K165" s="1">
         <v>110</v>
       </c>
-      <c r="L165" s="4" t="s">
-        <v>276</v>
+      <c r="L165" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="M165" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -6991,8 +7762,11 @@
       <c r="K166" s="1">
         <v>60</v>
       </c>
-      <c r="L166" s="5" t="s">
-        <v>277</v>
+      <c r="L166" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="M166" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -7023,8 +7797,11 @@
       <c r="K167" s="1">
         <v>70</v>
       </c>
-      <c r="L167" s="4" t="s">
-        <v>279</v>
+      <c r="L167" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="M167" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -7055,8 +7832,11 @@
       <c r="K168" s="1">
         <v>147</v>
       </c>
-      <c r="L168" s="5" t="s">
-        <v>278</v>
+      <c r="L168" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="M168" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -7087,8 +7867,11 @@
       <c r="K169" s="1">
         <v>90</v>
       </c>
-      <c r="L169" s="4" t="s">
-        <v>274</v>
+      <c r="L169" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="M169" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7119,11 +7902,11 @@
       <c r="K170" s="1">
         <v>100</v>
       </c>
-      <c r="L170" s="11" t="s">
+      <c r="L170" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M170" s="9" t="s">
-        <v>107</v>
+      <c r="M170" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -7154,8 +7937,11 @@
       <c r="K171" s="1">
         <v>156</v>
       </c>
-      <c r="L171" s="4" t="s">
-        <v>283</v>
+      <c r="L171" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="M171" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -7186,8 +7972,11 @@
       <c r="K172" s="1">
         <v>80</v>
       </c>
-      <c r="L172" s="5" t="s">
-        <v>284</v>
+      <c r="L172" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="M172" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -7218,8 +8007,11 @@
       <c r="K173" s="1">
         <v>75</v>
       </c>
-      <c r="L173" s="4" t="s">
-        <v>285</v>
+      <c r="L173" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="M173" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -7250,8 +8042,11 @@
       <c r="K174" s="1">
         <v>121</v>
       </c>
-      <c r="L174" s="5" t="s">
-        <v>286</v>
+      <c r="L174" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="M174" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -7282,8 +8077,11 @@
       <c r="K175" s="1">
         <v>131</v>
       </c>
-      <c r="L175" s="4" t="s">
-        <v>287</v>
+      <c r="L175" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="M175" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -7314,8 +8112,11 @@
       <c r="K176" s="1">
         <v>98</v>
       </c>
-      <c r="L176" s="5" t="s">
-        <v>290</v>
+      <c r="L176" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M176" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -7346,8 +8147,11 @@
       <c r="K177" s="1">
         <v>132</v>
       </c>
-      <c r="L177" s="4" t="s">
-        <v>292</v>
+      <c r="L177" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="M177" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
@@ -7378,8 +8182,11 @@
       <c r="K178" s="1">
         <v>149</v>
       </c>
-      <c r="L178" s="5" t="s">
-        <v>288</v>
+      <c r="L178" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="M178" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
@@ -7410,8 +8217,11 @@
       <c r="K179" s="1">
         <v>89</v>
       </c>
-      <c r="L179" s="4" t="s">
-        <v>289</v>
+      <c r="L179" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="M179" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
@@ -7442,11 +8252,11 @@
       <c r="K180" s="1">
         <v>69</v>
       </c>
-      <c r="L180" s="11" t="s">
+      <c r="L180" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="M180" s="9" t="s">
-        <v>116</v>
+      <c r="M180" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -7477,8 +8287,11 @@
       <c r="K181" s="1">
         <v>50</v>
       </c>
-      <c r="L181" s="4" t="s">
-        <v>291</v>
+      <c r="L181" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M181" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -7509,8 +8322,11 @@
       <c r="K182" s="1">
         <v>134</v>
       </c>
-      <c r="L182" s="5" t="s">
-        <v>293</v>
+      <c r="L182" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="M182" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -7541,8 +8357,11 @@
       <c r="K183" s="1">
         <v>78</v>
       </c>
-      <c r="L183" s="4" t="s">
-        <v>294</v>
+      <c r="L183" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="M183" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -7573,8 +8392,11 @@
       <c r="K184" s="1">
         <v>145</v>
       </c>
-      <c r="L184" s="5" t="s">
-        <v>295</v>
+      <c r="L184" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="M184" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -7605,8 +8427,11 @@
       <c r="K185" s="1">
         <v>82</v>
       </c>
-      <c r="L185" s="4" t="s">
-        <v>296</v>
+      <c r="L185" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="M185" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -7637,8 +8462,11 @@
       <c r="K186" s="1">
         <v>175</v>
       </c>
-      <c r="L186" s="5" t="s">
-        <v>297</v>
+      <c r="L186" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="M186" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -7669,8 +8497,11 @@
       <c r="K187" s="1">
         <v>91</v>
       </c>
-      <c r="L187" s="4" t="s">
-        <v>298</v>
+      <c r="L187" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="M187" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -7701,8 +8532,11 @@
       <c r="K188" s="1">
         <v>150</v>
       </c>
-      <c r="L188" s="5" t="s">
-        <v>299</v>
+      <c r="L188" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="M188" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -7733,8 +8567,11 @@
       <c r="K189" s="1">
         <v>110</v>
       </c>
-      <c r="L189" s="4" t="s">
-        <v>300</v>
+      <c r="L189" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="M189" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -7765,8 +8602,11 @@
       <c r="K190" s="1">
         <v>60</v>
       </c>
-      <c r="L190" s="5" t="s">
-        <v>301</v>
+      <c r="L190" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="M190" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
@@ -7797,8 +8637,11 @@
       <c r="K191" s="1">
         <v>70</v>
       </c>
-      <c r="L191" s="4" t="s">
-        <v>302</v>
+      <c r="L191" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="M191" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
@@ -7829,11 +8672,14 @@
       <c r="K192" s="1">
         <v>147</v>
       </c>
-      <c r="L192" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L192" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="M192" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>191</v>
       </c>
@@ -7861,8 +8707,11 @@
       <c r="K193" s="1">
         <v>90</v>
       </c>
-      <c r="L193" s="4" t="s">
-        <v>304</v>
+      <c r="L193" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="M193" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -7871,6 +8720,7 @@
       <dataRef ref="B1:K1048576" sheet="Sheet1"/>
     </dataRefs>
   </dataConsolidate>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>